<commit_message>
Data Science Interview Guide.xlsx
Data Science Interview Guide.xlsx
</commit_message>
<xml_diff>
--- a/Data Science Interview Guide.xlsx
+++ b/Data Science Interview Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siva\Desktop\LinkedIn\Data Science Career Path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95E78AB-2C29-4F8C-B5AB-57283EC50017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F18E3C2-14F0-4DF7-A90F-FB19FF5F97E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="167">
   <si>
     <t xml:space="preserve">This is a data science study guide that you can use to help prepare yourself for your interview. This was developed by people who have interviewed and gotten jobs at Amazon, Facebook, Capital One and several other tech companies. We hope these help you get great jobs as well.
 In order to use this, you can make a copy of this sheet and follow along with the study guide. Keeping track helps you know where you are and how you are doing.
@@ -515,9 +515,6 @@
     <t>Introduction</t>
   </si>
   <si>
-    <t>Prepared by Sivasubramanian</t>
-  </si>
-  <si>
     <t>www.linkedin.com/in/iamsivab</t>
   </si>
   <si>
@@ -525,13 +522,22 @@
   </si>
   <si>
     <t>Best of Luck!</t>
+  </si>
+  <si>
+    <t>Curated by Sivasubramanian</t>
+  </si>
+  <si>
+    <t>Created by https://www.linkedin.com/in/benjaminrogojan/</t>
+  </si>
+  <si>
+    <t>https://medium.com/better-programming/the-data-science-interview-study-guide-c3824cb76c2e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -617,8 +623,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -639,7 +661,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,7 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -746,6 +774,12 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1078,14 +1112,14 @@
   <dimension ref="A1:D1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="60.28515625" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="80.28515625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1098,7 +1132,7 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2675,98 +2709,107 @@
     </row>
     <row r="214" spans="1:3" ht="12.75">
       <c r="A214" s="24"/>
+      <c r="C214" s="29"/>
     </row>
     <row r="215" spans="1:3" ht="12.75">
       <c r="A215" s="24"/>
+      <c r="C215" s="29" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="216" spans="1:3" ht="12.75">
       <c r="A216" s="24"/>
+      <c r="C216" s="29"/>
     </row>
     <row r="217" spans="1:3" ht="12.75">
       <c r="A217" s="24"/>
+      <c r="C217" s="30" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="218" spans="1:3" ht="12.75">
       <c r="A218" s="24"/>
-      <c r="C218" s="25" t="s">
-        <v>161</v>
+      <c r="C218" s="29" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="12.75">
       <c r="A219" s="24"/>
-      <c r="C219" s="26"/>
+      <c r="C219" s="29"/>
     </row>
     <row r="220" spans="1:3" ht="12.75">
       <c r="A220" s="24"/>
-      <c r="C220" s="27" t="s">
-        <v>162</v>
+      <c r="C220" s="30" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="12.75">
       <c r="A221" s="24"/>
-      <c r="C221" s="26"/>
+      <c r="C221" s="29"/>
     </row>
     <row r="222" spans="1:3" ht="12.75">
       <c r="A222" s="24"/>
-      <c r="C222" s="26" t="s">
-        <v>163</v>
+      <c r="C222" s="29" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="12.75">
       <c r="A223" s="24"/>
-      <c r="C223" s="26"/>
+      <c r="C223" s="29"/>
     </row>
     <row r="224" spans="1:3" ht="12.75">
       <c r="A224" s="24"/>
-      <c r="C224" s="26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" ht="12.75">
+      <c r="C224" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="12.75">
       <c r="A225" s="24"/>
     </row>
-    <row r="226" spans="1:1" ht="12.75">
+    <row r="226" spans="1:3" ht="12.75">
       <c r="A226" s="24"/>
     </row>
-    <row r="227" spans="1:1" ht="12.75">
+    <row r="227" spans="1:3" ht="12.75">
       <c r="A227" s="24"/>
     </row>
-    <row r="228" spans="1:1" ht="12.75">
+    <row r="228" spans="1:3" ht="12.75">
       <c r="A228" s="24"/>
-    </row>
-    <row r="229" spans="1:1" ht="12.75">
+      <c r="C228" s="28"/>
+    </row>
+    <row r="229" spans="1:3" ht="12.75">
       <c r="A229" s="24"/>
     </row>
-    <row r="230" spans="1:1" ht="12.75">
+    <row r="230" spans="1:3" ht="12.75">
       <c r="A230" s="24"/>
     </row>
-    <row r="231" spans="1:1" ht="12.75">
+    <row r="231" spans="1:3" ht="12.75">
       <c r="A231" s="24"/>
     </row>
-    <row r="232" spans="1:1" ht="12.75">
+    <row r="232" spans="1:3" ht="12.75">
       <c r="A232" s="24"/>
     </row>
-    <row r="233" spans="1:1" ht="12.75">
+    <row r="233" spans="1:3" ht="12.75">
       <c r="A233" s="24"/>
     </row>
-    <row r="234" spans="1:1" ht="12.75">
+    <row r="234" spans="1:3" ht="12.75">
       <c r="A234" s="24"/>
     </row>
-    <row r="235" spans="1:1" ht="12.75">
+    <row r="235" spans="1:3" ht="12.75">
       <c r="A235" s="24"/>
     </row>
-    <row r="236" spans="1:1" ht="12.75">
+    <row r="236" spans="1:3" ht="12.75">
       <c r="A236" s="24"/>
     </row>
-    <row r="237" spans="1:1" ht="12.75">
+    <row r="237" spans="1:3" ht="12.75">
       <c r="A237" s="24"/>
     </row>
-    <row r="238" spans="1:1" ht="12.75">
+    <row r="238" spans="1:3" ht="12.75">
       <c r="A238" s="24"/>
     </row>
-    <row r="239" spans="1:1" ht="12.75">
+    <row r="239" spans="1:3" ht="12.75">
       <c r="A239" s="24"/>
     </row>
-    <row r="240" spans="1:1" ht="12.75">
+    <row r="240" spans="1:3" ht="12.75">
       <c r="A240" s="24"/>
     </row>
     <row r="241" spans="1:1" ht="12.75">
@@ -3034,33 +3077,25 @@
       <c r="A328" s="24"/>
     </row>
     <row r="329" spans="1:1" ht="12.75">
-      <c r="A329" s="25" t="s">
-        <v>161</v>
-      </c>
+      <c r="A329" s="25"/>
     </row>
     <row r="330" spans="1:1" ht="12.75">
       <c r="A330" s="26"/>
     </row>
     <row r="331" spans="1:1" ht="12.75">
-      <c r="A331" s="27" t="s">
-        <v>162</v>
-      </c>
+      <c r="A331" s="27"/>
     </row>
     <row r="332" spans="1:1" ht="12.75">
       <c r="A332" s="26"/>
     </row>
     <row r="333" spans="1:1" ht="12.75">
-      <c r="A333" s="26" t="s">
-        <v>163</v>
-      </c>
+      <c r="A333" s="26"/>
     </row>
     <row r="334" spans="1:1" ht="12.75">
       <c r="A334" s="26"/>
     </row>
     <row r="335" spans="1:1" ht="12.75">
-      <c r="A335" s="26" t="s">
-        <v>164</v>
-      </c>
+      <c r="A335" s="26"/>
     </row>
     <row r="336" spans="1:1" ht="12.75">
       <c r="A336" s="24"/>
@@ -3457,9 +3492,7 @@
     </row>
     <row r="467" spans="1:3" ht="12.75">
       <c r="A467" s="24"/>
-      <c r="C467" s="25" t="s">
-        <v>161</v>
-      </c>
+      <c r="C467" s="25"/>
     </row>
     <row r="468" spans="1:3" ht="12.75">
       <c r="A468" s="24"/>
@@ -3467,9 +3500,7 @@
     </row>
     <row r="469" spans="1:3" ht="12.75">
       <c r="A469" s="24"/>
-      <c r="C469" s="27" t="s">
-        <v>162</v>
-      </c>
+      <c r="C469" s="27"/>
     </row>
     <row r="470" spans="1:3" ht="12.75">
       <c r="A470" s="24"/>
@@ -3477,9 +3508,7 @@
     </row>
     <row r="471" spans="1:3" ht="12.75">
       <c r="A471" s="24"/>
-      <c r="C471" s="26" t="s">
-        <v>163</v>
-      </c>
+      <c r="C471" s="26"/>
     </row>
     <row r="472" spans="1:3" ht="12.75">
       <c r="A472" s="24"/>
@@ -3487,9 +3516,7 @@
     </row>
     <row r="473" spans="1:3" ht="12.75">
       <c r="A473" s="24"/>
-      <c r="C473" s="26" t="s">
-        <v>164</v>
-      </c>
+      <c r="C473" s="26"/>
     </row>
     <row r="474" spans="1:3" ht="12.75">
       <c r="A474" s="24"/>
@@ -3624,33 +3651,25 @@
       <c r="A517" s="24"/>
     </row>
     <row r="518" spans="1:1" ht="12.75">
-      <c r="A518" s="25" t="s">
-        <v>161</v>
-      </c>
+      <c r="A518" s="25"/>
     </row>
     <row r="519" spans="1:1" ht="12.75">
       <c r="A519" s="26"/>
     </row>
     <row r="520" spans="1:1" ht="12.75">
-      <c r="A520" s="27" t="s">
-        <v>162</v>
-      </c>
+      <c r="A520" s="27"/>
     </row>
     <row r="521" spans="1:1" ht="12.75">
       <c r="A521" s="26"/>
     </row>
     <row r="522" spans="1:1" ht="12.75">
-      <c r="A522" s="26" t="s">
-        <v>163</v>
-      </c>
+      <c r="A522" s="26"/>
     </row>
     <row r="523" spans="1:1" ht="12.75">
       <c r="A523" s="26"/>
     </row>
     <row r="524" spans="1:1" ht="12.75">
-      <c r="A524" s="26" t="s">
-        <v>164</v>
-      </c>
+      <c r="A524" s="26"/>
     </row>
     <row r="525" spans="1:1" ht="12.75">
       <c r="A525" s="24"/>
@@ -5250,11 +5269,9 @@
     <hyperlink ref="A203" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
     <hyperlink ref="A204" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
     <hyperlink ref="C220" r:id="rId114" xr:uid="{7CDC3A63-F818-4778-828C-DDC430FE664A}"/>
-    <hyperlink ref="A331" r:id="rId115" xr:uid="{52CF40E9-CEA8-4E8D-BE2C-33E6B7CD03FF}"/>
-    <hyperlink ref="C469" r:id="rId116" xr:uid="{79E02615-A0BE-4911-AA5D-F4025BB2D1D4}"/>
-    <hyperlink ref="A520" r:id="rId117" xr:uid="{9D5951A7-3245-4C43-9EFE-1AF22447BD53}"/>
+    <hyperlink ref="C217" r:id="rId115" xr:uid="{5E38A8FA-FB45-40D8-B9E3-8855E58D3CD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId118"/>
+  <pageSetup orientation="portrait" r:id="rId116"/>
 </worksheet>
 </file>
</xml_diff>